<commit_message>
ADD test cases for grinko
</commit_message>
<xml_diff>
--- a/Template_test_cases_grinko.xlsx
+++ b/Template_test_cases_grinko.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\skillup1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="312" windowWidth="15132" windowHeight="7380" tabRatio="861" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="315" windowWidth="15135" windowHeight="7380" tabRatio="861" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="21" r:id="rId1"/>
@@ -22,12 +27,12 @@
     <definedName name="Citing_Articles">'[3]General Search'!$B$9:$B$14</definedName>
     <definedName name="Results">'[4]General Search'!$B$9:$B$14</definedName>
   </definedNames>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
   <si>
     <r>
       <t>How the tree directory is structured in Quality Center</t>
@@ -200,11 +205,137 @@
   <si>
     <t>INCI-2102</t>
   </si>
+  <si>
+    <t>Tab 'Edit'</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Notepad is opened.</t>
+  </si>
+  <si>
+    <t>Click tab 'Edit'</t>
+  </si>
+  <si>
+    <t>Drop-down list is opened.</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Write down text into text field</t>
+  </si>
+  <si>
+    <t>Click 'Edit' tab</t>
+  </si>
+  <si>
+    <t>qwerty</t>
+  </si>
+  <si>
+    <t>NP_EDIT_001</t>
+  </si>
+  <si>
+    <t>NP_EDIT_002</t>
+  </si>
+  <si>
+    <t>NP_EDIT_003</t>
+  </si>
+  <si>
+    <t>Drop-down list elements verification while text is written.</t>
+  </si>
+  <si>
+    <t>Drop-down list verification.</t>
+  </si>
+  <si>
+    <t>Drop-down list elements verification while text is not written.</t>
+  </si>
+  <si>
+    <t>Keep text field blank</t>
+  </si>
+  <si>
+    <t>NP_EDIT_004</t>
+  </si>
+  <si>
+    <t>Notepad is opened. Text is written.</t>
+  </si>
+  <si>
+    <t>Highlight text in text field</t>
+  </si>
+  <si>
+    <t>Click 'Cut'</t>
+  </si>
+  <si>
+    <t>Text is cut into draft.</t>
+  </si>
+  <si>
+    <t>Undo', 'Replace', 'Select All', 'Time/Date' elements are available.</t>
+  </si>
+  <si>
+    <t>Undo', 'Find…', 'Find next', 'Replace', 'Select All', 'Time/Date' elements are available.</t>
+  </si>
+  <si>
+    <t>NP_EDIT_005</t>
+  </si>
+  <si>
+    <t>Click 'Copy'</t>
+  </si>
+  <si>
+    <t>NP_EDIT_006</t>
+  </si>
+  <si>
+    <t>Notepad is opened. Text is drafted.</t>
+  </si>
+  <si>
+    <t>Paste' element verification.</t>
+  </si>
+  <si>
+    <t>Copy' element verification.</t>
+  </si>
+  <si>
+    <t>Cut' element verification.</t>
+  </si>
+  <si>
+    <t>Click 'Paste'</t>
+  </si>
+  <si>
+    <t>NP_EDIT_007</t>
+  </si>
+  <si>
+    <t>Delete' element verification</t>
+  </si>
+  <si>
+    <t>Click 'Delete'</t>
+  </si>
+  <si>
+    <t>Text is deleted.</t>
+  </si>
+  <si>
+    <t>Text is pasted into text field.</t>
+  </si>
+  <si>
+    <t>Text is copied into draft.</t>
+  </si>
+  <si>
+    <t>NP_EDIT_008</t>
+  </si>
+  <si>
+    <t>Notepad is opened</t>
+  </si>
+  <si>
+    <t>Time/Date' element verification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click 'Time/Date' </t>
+  </si>
+  <si>
+    <t>Actual time and date are pasted into text field.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -314,7 +445,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -358,38 +489,6 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -400,10 +499,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Hyperlink 3" xfId="1"/>
     <cellStyle name="Hyperlink 4" xfId="2"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 18" xfId="3"/>
     <cellStyle name="Normal 4 3" xfId="4"/>
     <cellStyle name="Normal 8 3" xfId="5"/>
@@ -411,7 +520,6 @@
     <cellStyle name="Normal 8 5" xfId="7"/>
     <cellStyle name="Normal 8 6" xfId="8"/>
     <cellStyle name="Normal_webofscience checklist" xfId="9"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="40">
     <dxf>
@@ -768,7 +876,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -842,7 +950,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -916,7 +1024,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -966,7 +1074,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FSTA"/>
@@ -1016,9 +1124,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1056,9 +1164,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1090,9 +1198,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1124,9 +1233,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1299,133 +1409,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="106.6640625" customWidth="1"/>
+    <col min="1" max="1" width="106.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="25"/>
+      <c r="A2" s="16"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="25"/>
+      <c r="A3" s="16"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="25"/>
+      <c r="A4" s="16"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="25"/>
+      <c r="A5" s="16"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="25"/>
+      <c r="A6" s="16"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="25"/>
+      <c r="A7" s="16"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="25"/>
+      <c r="A8" s="16"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="25"/>
+      <c r="A9" s="16"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="25"/>
+      <c r="A10" s="16"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="25"/>
+      <c r="A11" s="16"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="25"/>
+      <c r="A12" s="16"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="25"/>
+      <c r="A13" s="16"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="25"/>
+      <c r="A14" s="16"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="25"/>
+      <c r="A15" s="16"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="25"/>
+      <c r="A16" s="16"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="25"/>
+      <c r="A17" s="16"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="25"/>
+      <c r="A18" s="16"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="25"/>
+      <c r="A19" s="16"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="25"/>
+      <c r="A20" s="16"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="25"/>
+      <c r="A21" s="16"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="25"/>
+      <c r="A22" s="16"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="25"/>
+      <c r="A23" s="16"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="25"/>
+      <c r="A24" s="16"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="25"/>
+      <c r="A25" s="16"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="25"/>
+      <c r="A26" s="16"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="25"/>
+      <c r="A27" s="16"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="25"/>
+      <c r="A28" s="16"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="25"/>
+      <c r="A29" s="16"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="25"/>
+      <c r="A30" s="16"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="25"/>
+      <c r="A31" s="16"/>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="25"/>
+      <c r="A32" s="16"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="25"/>
+      <c r="A33" s="16"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="25"/>
+      <c r="A34" s="16"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="25"/>
+      <c r="A35" s="16"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="25"/>
+      <c r="A36" s="16"/>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="25"/>
+      <c r="A37" s="16"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="25"/>
+      <c r="A38" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1438,28 +1548,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="10"/>
-    <col min="3" max="3" width="9.6640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="33.44140625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="11"/>
+    <col min="1" max="2" width="9.140625" style="10"/>
+    <col min="3" max="3" width="9.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="11"/>
     <col min="7" max="7" width="62" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="63.5546875" style="10" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="10"/>
+    <col min="8" max="8" width="14.28515625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="63.5703125" style="10" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="12" customFormat="1" ht="66">
+    <row r="1" spans="1:19" s="12" customFormat="1" ht="63.75">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -1518,7 +1628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="52.8">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="51">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -1537,7 +1647,7 @@
       <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="13" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="4"/>
@@ -1582,10 +1692,10 @@
       <c r="R3" s="9"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="1:19" s="12" customFormat="1" ht="26.4">
+    <row r="4" spans="1:19" s="12" customFormat="1" ht="25.5">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="23"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
       <c r="F4" s="3">
@@ -1611,194 +1721,582 @@
       <c r="R4" s="9"/>
       <c r="S4" s="7"/>
     </row>
-    <row r="5" spans="1:19" s="12" customFormat="1">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="14"/>
-    </row>
-    <row r="6" spans="1:19" s="12" customFormat="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="14"/>
+    <row r="5" spans="1:19" s="12" customFormat="1" ht="25.5">
+      <c r="A5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="7"/>
+    </row>
+    <row r="6" spans="1:19" s="12" customFormat="1" ht="25.5">
+      <c r="A6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="7"/>
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="14"/>
-    </row>
-    <row r="8" spans="1:19" s="12" customFormat="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="14"/>
-    </row>
-    <row r="9" spans="1:19" s="12" customFormat="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="14"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="7"/>
+    </row>
+    <row r="8" spans="1:19" s="12" customFormat="1" ht="25.5">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="7"/>
+    </row>
+    <row r="9" spans="1:19" s="12" customFormat="1" ht="25.5">
+      <c r="A9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="14"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="3">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="14"/>
+      <c r="A11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" s="12" customFormat="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="14"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" s="12" customFormat="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="14"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="3">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="7"/>
+    </row>
+    <row r="14" spans="1:19" ht="25.5">
+      <c r="A14" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="19">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="19">
+        <v>2</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="19">
+        <v>3</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+    </row>
+    <row r="17" spans="1:19" ht="25.5">
+      <c r="A17" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="19">
+        <v>1</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="19">
+        <v>2</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+    </row>
+    <row r="19" spans="1:19" ht="25.5">
+      <c r="A19" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="19">
+        <v>2</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="19">
+        <v>3</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+    </row>
+    <row r="22" spans="1:19" ht="25.5">
+      <c r="A22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="19">
+        <v>1</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="19">
+        <v>2</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I4 G4:G6 I12:I13 G12:G13">

</xml_diff>